<commit_message>
removed MS4- from weir_dims
</commit_message>
<xml_diff>
--- a/Ancillary_files/Weir Dims 2020.xlsx
+++ b/Ancillary_files/Weir Dims 2020.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
   <si>
     <t>Site</t>
   </si>
@@ -224,130 +224,61 @@
     <t>c2= edge of wing to inside of pipe wall</t>
   </si>
   <si>
-    <t>MS4-CAR-007</t>
-  </si>
-  <si>
-    <t>MS4-CAR-059</t>
-  </si>
-  <si>
-    <t>MS4-CAR-059G</t>
-  </si>
-  <si>
-    <t>MS4-CAR-070</t>
-  </si>
-  <si>
-    <t>MS4-CAR-070E</t>
-  </si>
-  <si>
-    <t>MS4-CAR-072</t>
-  </si>
-  <si>
-    <t>MS4-CAR-072C</t>
-  </si>
-  <si>
-    <t>MS4-CAR-072R</t>
-  </si>
-  <si>
-    <t>MS4-CAR-072O</t>
-  </si>
-  <si>
-    <t>MS4-CAR-072Q</t>
-  </si>
-  <si>
-    <t>MS4-SDG-072</t>
-  </si>
-  <si>
-    <t>MS4-SDG-072A</t>
-  </si>
-  <si>
-    <t>MS4-SDG-084</t>
-  </si>
-  <si>
-    <t>MS4-SDG-084J</t>
-  </si>
-  <si>
-    <t>MS4-SDG-085</t>
-  </si>
-  <si>
-    <t>MS4-SDG-085G</t>
-  </si>
-  <si>
-    <t>MS4-SDG-085M</t>
-  </si>
-  <si>
-    <t>MS4-SDR-036</t>
-  </si>
-  <si>
-    <t>MS4-SDR-041</t>
-  </si>
-  <si>
-    <t>MS4-SDR-064</t>
-  </si>
-  <si>
-    <t>MS4-SDR-064A</t>
-  </si>
-  <si>
-    <t>MS4-SDR-064B</t>
-  </si>
-  <si>
-    <t>MS4-SDR-064C</t>
-  </si>
-  <si>
-    <t>MS4-SDR-064D</t>
-  </si>
-  <si>
-    <t>MS4-SDR-098</t>
-  </si>
-  <si>
-    <t>MS4-SDR-127</t>
-  </si>
-  <si>
-    <t>MS4-SDR-127B</t>
-  </si>
-  <si>
-    <t>MS4-SDR-130</t>
-  </si>
-  <si>
-    <t>MS4-SDR-203A</t>
-  </si>
-  <si>
-    <t>MS4-SDR-204A</t>
-  </si>
-  <si>
-    <t>MS4-SLR-045</t>
-  </si>
-  <si>
-    <t>MS4-SLR-045A</t>
-  </si>
-  <si>
-    <t>MS4-SLR-045B</t>
-  </si>
-  <si>
-    <t>MS4-SLR-095</t>
-  </si>
-  <si>
-    <t>MS4-SWT-019</t>
-  </si>
-  <si>
-    <t>MS4-SWT-030</t>
-  </si>
-  <si>
-    <t>MS4-SWT-030I</t>
-  </si>
-  <si>
-    <t>MS4-SWT-068</t>
-  </si>
-  <si>
-    <t>MS4-SWT-162</t>
-  </si>
-  <si>
-    <t>MS4-SWT-233</t>
-  </si>
-  <si>
-    <t>MS4-SWT-235</t>
-  </si>
-  <si>
     <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>CAR-007</t>
+  </si>
+  <si>
+    <t>CAR-059</t>
+  </si>
+  <si>
+    <t>CAR-059G</t>
+  </si>
+  <si>
+    <t>CAR-070E</t>
+  </si>
+  <si>
+    <t>CAR-072C</t>
+  </si>
+  <si>
+    <t>CAR-072R</t>
+  </si>
+  <si>
+    <t>CAR-072Q</t>
+  </si>
+  <si>
+    <t>SDG-072A</t>
+  </si>
+  <si>
+    <t>SDR-064A</t>
+  </si>
+  <si>
+    <t>SDR-064B</t>
+  </si>
+  <si>
+    <t>SDR-064C</t>
+  </si>
+  <si>
+    <t>SDR-064D</t>
+  </si>
+  <si>
+    <t>SDR-130</t>
+  </si>
+  <si>
+    <t>SWT-030I</t>
+  </si>
+  <si>
+    <t>SWT-068</t>
+  </si>
+  <si>
+    <t>SWT-162</t>
+  </si>
+  <si>
+    <t>SWT-233</t>
+  </si>
+  <si>
+    <t>SWT-235</t>
   </si>
 </sst>
 </file>
@@ -2286,10 +2217,10 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:I43"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2356,8 +2287,8 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>62</v>
+      <c r="A3" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="27">
         <v>43956</v>
@@ -2386,38 +2317,38 @@
       <c r="J3" s="22"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>63</v>
+      <c r="A4" t="s">
+        <v>64</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J4" s="22"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>64</v>
+      <c r="A5" t="s">
+        <v>65</v>
       </c>
       <c r="B5" s="27">
         <v>43956</v>
@@ -2446,8 +2377,8 @@
       <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>65</v>
+      <c r="A6" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="27">
         <v>43952</v>
@@ -2476,7 +2407,7 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="27">
@@ -2506,8 +2437,8 @@
       <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>67</v>
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="27">
         <v>43952</v>
@@ -2536,8 +2467,8 @@
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>68</v>
+      <c r="A9" t="s">
+        <v>67</v>
       </c>
       <c r="B9" s="27">
         <v>43964</v>
@@ -2566,8 +2497,8 @@
       <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>69</v>
+      <c r="A10" t="s">
+        <v>68</v>
       </c>
       <c r="B10" s="27">
         <v>43964</v>
@@ -2596,8 +2527,8 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
-        <v>70</v>
+      <c r="A11" t="s">
+        <v>49</v>
       </c>
       <c r="B11" s="27">
         <v>43964</v>
@@ -2626,8 +2557,8 @@
       <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>71</v>
+      <c r="A12" t="s">
+        <v>69</v>
       </c>
       <c r="B12" s="27">
         <v>43964</v>
@@ -2656,8 +2587,8 @@
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
-        <v>72</v>
+      <c r="A13" t="s">
+        <v>43</v>
       </c>
       <c r="B13" s="27">
         <v>43956</v>
@@ -2686,8 +2617,8 @@
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
-        <v>73</v>
+      <c r="A14" t="s">
+        <v>70</v>
       </c>
       <c r="B14" s="27">
         <v>43963</v>
@@ -2716,8 +2647,8 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>74</v>
+      <c r="A15" t="s">
+        <v>44</v>
       </c>
       <c r="B15" s="27">
         <v>43956</v>
@@ -2746,8 +2677,8 @@
       <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
-        <v>75</v>
+      <c r="A16" t="s">
+        <v>11</v>
       </c>
       <c r="B16" s="27">
         <v>43963</v>
@@ -2776,8 +2707,8 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
-        <v>76</v>
+      <c r="A17" t="s">
+        <v>45</v>
       </c>
       <c r="B17" s="27">
         <v>43956</v>
@@ -2806,8 +2737,8 @@
       <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
-        <v>77</v>
+      <c r="A18" t="s">
+        <v>46</v>
       </c>
       <c r="B18" s="27">
         <v>43963</v>
@@ -2836,8 +2767,8 @@
       <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
-        <v>78</v>
+      <c r="A19" t="s">
+        <v>12</v>
       </c>
       <c r="B19" s="27">
         <v>43963</v>
@@ -2852,22 +2783,22 @@
         <v>12</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G19" s="28">
         <v>6</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
-        <v>79</v>
+      <c r="A20" t="s">
+        <v>21</v>
       </c>
       <c r="B20" s="30">
         <v>43959</v>
@@ -2882,22 +2813,22 @@
         <v>12</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G20" s="28">
         <v>6</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
-        <v>80</v>
+      <c r="A21" t="s">
+        <v>42</v>
       </c>
       <c r="B21" s="30">
         <v>43959</v>
@@ -2926,8 +2857,8 @@
       <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
-        <v>81</v>
+      <c r="A22" t="s">
+        <v>33</v>
       </c>
       <c r="B22" s="30">
         <v>43959</v>
@@ -2942,22 +2873,22 @@
         <v>10</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G22" s="28">
         <v>5</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I22" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>82</v>
+      <c r="A23" t="s">
+        <v>71</v>
       </c>
       <c r="B23" s="30">
         <v>43959</v>
@@ -2986,8 +2917,8 @@
       <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="24" t="s">
-        <v>83</v>
+      <c r="A24" t="s">
+        <v>72</v>
       </c>
       <c r="B24" s="30">
         <v>43959</v>
@@ -3002,22 +2933,22 @@
         <v>12</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G24" s="28">
         <v>6</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I24" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="24" t="s">
-        <v>84</v>
+      <c r="A25" t="s">
+        <v>73</v>
       </c>
       <c r="B25" s="30">
         <v>43959</v>
@@ -3032,22 +2963,22 @@
         <v>12</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G25" s="28">
         <v>6</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I25" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J25" s="22"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="24" t="s">
-        <v>85</v>
+      <c r="A26" t="s">
+        <v>74</v>
       </c>
       <c r="B26" s="30">
         <v>43959</v>
@@ -3076,8 +3007,8 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
-        <v>86</v>
+      <c r="A27" t="s">
+        <v>23</v>
       </c>
       <c r="B27" s="30">
         <v>43959</v>
@@ -3106,8 +3037,8 @@
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="24" t="s">
-        <v>87</v>
+      <c r="A28" t="s">
+        <v>32</v>
       </c>
       <c r="B28" s="30">
         <v>43959</v>
@@ -3136,8 +3067,8 @@
       <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="24" t="s">
-        <v>88</v>
+      <c r="A29" t="s">
+        <v>53</v>
       </c>
       <c r="B29" s="30">
         <v>43959</v>
@@ -3166,8 +3097,8 @@
       <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
-        <v>89</v>
+      <c r="A30" t="s">
+        <v>75</v>
       </c>
       <c r="B30" s="30">
         <v>43959</v>
@@ -3196,8 +3127,8 @@
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>90</v>
+      <c r="A31" t="s">
+        <v>29</v>
       </c>
       <c r="B31" s="30">
         <v>43959</v>
@@ -3226,8 +3157,8 @@
       <c r="J31" s="22"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="24" t="s">
-        <v>91</v>
+      <c r="A32" t="s">
+        <v>30</v>
       </c>
       <c r="B32" s="30">
         <v>43959</v>
@@ -3256,8 +3187,8 @@
       <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
-        <v>92</v>
+      <c r="A33" t="s">
+        <v>16</v>
       </c>
       <c r="B33" s="27">
         <v>43952</v>
@@ -3286,8 +3217,8 @@
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="24" t="s">
-        <v>93</v>
+      <c r="A34" t="s">
+        <v>15</v>
       </c>
       <c r="B34" s="27">
         <v>43952</v>
@@ -3316,8 +3247,8 @@
       <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
-        <v>94</v>
+      <c r="A35" t="s">
+        <v>13</v>
       </c>
       <c r="B35" s="27">
         <v>43952</v>
@@ -3332,22 +3263,22 @@
         <v>12</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G35" s="28">
         <v>6</v>
       </c>
       <c r="H35" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="24" t="s">
-        <v>95</v>
+      <c r="A36" t="s">
+        <v>47</v>
       </c>
       <c r="B36" s="27">
         <v>43952</v>
@@ -3376,8 +3307,8 @@
       <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
-        <v>96</v>
+      <c r="A37" t="s">
+        <v>20</v>
       </c>
       <c r="B37" s="27">
         <v>43958</v>
@@ -3406,8 +3337,8 @@
       <c r="J37" s="22"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>97</v>
+      <c r="A38" t="s">
+        <v>24</v>
       </c>
       <c r="B38" s="27">
         <v>43958</v>
@@ -3436,8 +3367,8 @@
       <c r="J38" s="22"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
-        <v>98</v>
+      <c r="A39" t="s">
+        <v>76</v>
       </c>
       <c r="B39" s="27">
         <v>43958</v>
@@ -3466,8 +3397,8 @@
       <c r="J39" s="22"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
-        <v>99</v>
+      <c r="A40" t="s">
+        <v>77</v>
       </c>
       <c r="B40" s="27">
         <v>43958</v>
@@ -3482,22 +3413,22 @@
         <v>8</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G40" s="28">
         <v>4</v>
       </c>
       <c r="H40" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I40" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="J40" s="22"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
-        <v>100</v>
+      <c r="A41" t="s">
+        <v>78</v>
       </c>
       <c r="B41" s="27">
         <v>43958</v>
@@ -3526,8 +3457,8 @@
       <c r="J41" s="22"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="24" t="s">
-        <v>101</v>
+      <c r="A42" t="s">
+        <v>79</v>
       </c>
       <c r="B42" s="27">
         <v>43958</v>
@@ -3556,8 +3487,8 @@
       <c r="J42" s="22"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="24" t="s">
-        <v>102</v>
+      <c r="A43" t="s">
+        <v>80</v>
       </c>
       <c r="B43" s="27">
         <v>43958</v>
@@ -3572,16 +3503,16 @@
         <v>11.5</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="G43" s="24">
         <v>5.75</v>
       </c>
       <c r="H43" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="I43" s="34" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
getting data ready for July deliverable
</commit_message>
<xml_diff>
--- a/Ancillary_files/Weir Dims 2020.xlsx
+++ b/Ancillary_files/Weir Dims 2020.xlsx
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2019'!$A$2:$I$24</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020'!$A$2:$I$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020'!$A$2:$I$25</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="83">
   <si>
     <t>Site</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>SWT-235</t>
+  </si>
+  <si>
+    <t>SDG-287</t>
+  </si>
+  <si>
+    <t>b2 should equal 2 x h2</t>
   </si>
 </sst>
 </file>
@@ -2214,13 +2220,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31:XFD31"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="A20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,7 +2253,7 @@
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="25" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>60</v>
@@ -2798,25 +2804,25 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="30">
-        <v>43959</v>
+        <v>81</v>
+      </c>
+      <c r="B20" s="27">
+        <v>44040</v>
       </c>
       <c r="C20" s="28">
+        <v>3</v>
+      </c>
+      <c r="D20" s="31">
+        <v>4</v>
+      </c>
+      <c r="E20" s="28">
         <v>16</v>
-      </c>
-      <c r="D20" s="31">
-        <v>16</v>
-      </c>
-      <c r="E20" s="28">
-        <v>12</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>62</v>
       </c>
       <c r="G20" s="28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>62</v>
@@ -2828,136 +2834,136 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B21" s="30">
         <v>43959</v>
       </c>
       <c r="C21" s="28">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D21" s="31">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E21" s="28">
         <v>12</v>
       </c>
-      <c r="F21" s="28">
-        <v>2</v>
+      <c r="F21" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="G21" s="28">
         <v>6</v>
       </c>
-      <c r="H21" s="28">
-        <v>7</v>
-      </c>
-      <c r="I21" s="28">
-        <v>12</v>
+      <c r="H21" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B22" s="30">
         <v>43959</v>
       </c>
-      <c r="C22" s="32">
-        <v>36</v>
-      </c>
-      <c r="D22" s="32">
-        <v>36</v>
-      </c>
-      <c r="E22" s="32">
-        <v>10</v>
-      </c>
-      <c r="F22" s="34" t="s">
-        <v>62</v>
+      <c r="C22" s="28">
+        <v>6</v>
+      </c>
+      <c r="D22" s="31">
+        <v>6</v>
+      </c>
+      <c r="E22" s="28">
+        <v>12</v>
+      </c>
+      <c r="F22" s="28">
+        <v>2</v>
       </c>
       <c r="G22" s="28">
-        <v>5</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>62</v>
+        <v>6</v>
+      </c>
+      <c r="H22" s="28">
+        <v>7</v>
+      </c>
+      <c r="I22" s="28">
+        <v>12</v>
       </c>
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="B23" s="30">
         <v>43959</v>
       </c>
-      <c r="C23" s="28">
-        <v>4.5</v>
-      </c>
-      <c r="D23" s="28">
-        <v>4.75</v>
-      </c>
-      <c r="E23" s="28">
-        <v>8</v>
-      </c>
-      <c r="F23" s="28">
-        <v>2</v>
+      <c r="C23" s="32">
+        <v>36</v>
+      </c>
+      <c r="D23" s="32">
+        <v>36</v>
+      </c>
+      <c r="E23" s="32">
+        <v>10</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="G23" s="28">
-        <v>4</v>
-      </c>
-      <c r="H23" s="28">
-        <v>1</v>
-      </c>
-      <c r="I23" s="28">
-        <v>0.5</v>
+        <v>5</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="30">
         <v>43959</v>
       </c>
       <c r="C24" s="28">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="D24" s="28">
-        <v>3</v>
-      </c>
-      <c r="E24" s="32">
-        <v>12</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>62</v>
+        <v>4.75</v>
+      </c>
+      <c r="E24" s="28">
+        <v>8</v>
+      </c>
+      <c r="F24" s="28">
+        <v>2</v>
       </c>
       <c r="G24" s="28">
-        <v>6</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I24" s="34" t="s">
-        <v>62</v>
+        <v>4</v>
+      </c>
+      <c r="H24" s="28">
+        <v>1</v>
+      </c>
+      <c r="I24" s="28">
+        <v>0.5</v>
       </c>
       <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25" s="30">
         <v>43959</v>
       </c>
       <c r="C25" s="28">
-        <v>7</v>
+        <v>3.5</v>
       </c>
       <c r="D25" s="28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E25" s="32">
         <v>12</v>
@@ -2978,136 +2984,136 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B26" s="30">
         <v>43959</v>
       </c>
       <c r="C26" s="28">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D26" s="28">
-        <v>4</v>
-      </c>
-      <c r="E26" s="28">
-        <v>12</v>
-      </c>
-      <c r="F26" s="28">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="E26" s="32">
+        <v>12</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="G26" s="28">
         <v>6</v>
       </c>
-      <c r="H26" s="28">
-        <v>6.25</v>
-      </c>
-      <c r="I26" s="28">
-        <v>4.25</v>
+      <c r="H26" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="B27" s="30">
         <v>43959</v>
       </c>
       <c r="C27" s="28">
-        <v>10</v>
-      </c>
-      <c r="D27" s="31">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="D27" s="28">
+        <v>4</v>
       </c>
       <c r="E27" s="28">
-        <v>9.75</v>
+        <v>12</v>
       </c>
       <c r="F27" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="28">
-        <v>5.25</v>
+        <v>6</v>
       </c>
       <c r="H27" s="28">
-        <v>12</v>
+        <v>6.25</v>
       </c>
       <c r="I27" s="28">
-        <v>12</v>
+        <v>4.25</v>
       </c>
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B28" s="30">
         <v>43959</v>
       </c>
       <c r="C28" s="28">
-        <v>15</v>
-      </c>
-      <c r="D28" s="28">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D28" s="31">
+        <v>10</v>
       </c>
       <c r="E28" s="28">
-        <v>10</v>
+        <v>9.75</v>
       </c>
       <c r="F28" s="28">
         <v>1</v>
       </c>
       <c r="G28" s="28">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="H28" s="28">
-        <v>9.75</v>
+        <v>12</v>
       </c>
       <c r="I28" s="28">
-        <v>15.75</v>
+        <v>12</v>
       </c>
       <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B29" s="30">
         <v>43959</v>
       </c>
       <c r="C29" s="28">
-        <v>6.75</v>
-      </c>
-      <c r="D29" s="31">
-        <v>6.5</v>
+        <v>15</v>
+      </c>
+      <c r="D29" s="28">
+        <v>15</v>
       </c>
       <c r="E29" s="28">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F29" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H29" s="28">
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="I29" s="28">
-        <v>7.25</v>
+        <v>15.75</v>
       </c>
       <c r="J29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B30" s="30">
         <v>43959</v>
       </c>
       <c r="C30" s="28">
-        <v>9</v>
+        <v>6.75</v>
       </c>
       <c r="D30" s="31">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="E30" s="28">
         <v>12</v>
@@ -3119,10 +3125,10 @@
         <v>6</v>
       </c>
       <c r="H30" s="28">
-        <v>4</v>
+        <v>9.5</v>
       </c>
       <c r="I30" s="28">
-        <v>4</v>
+        <v>7.25</v>
       </c>
       <c r="J30" s="22"/>
     </row>
@@ -3131,22 +3137,22 @@
         <v>75</v>
       </c>
       <c r="B31" s="30">
-        <v>43978</v>
+        <v>43959</v>
       </c>
       <c r="C31" s="28">
-        <v>10.75</v>
+        <v>9</v>
       </c>
       <c r="D31" s="31">
-        <v>10.75</v>
+        <v>9</v>
       </c>
       <c r="E31" s="28">
-        <v>17.5</v>
+        <v>12</v>
       </c>
       <c r="F31" s="28">
         <v>2</v>
       </c>
       <c r="G31" s="28">
-        <v>8.625</v>
+        <v>6</v>
       </c>
       <c r="H31" s="28">
         <v>4</v>
@@ -3158,196 +3164,196 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B32" s="30">
-        <v>43959</v>
+        <v>43978</v>
       </c>
       <c r="C32" s="28">
-        <v>10</v>
+        <v>10.75</v>
       </c>
       <c r="D32" s="31">
-        <v>10</v>
+        <v>10.75</v>
       </c>
       <c r="E32" s="28">
-        <v>12</v>
+        <v>17.5</v>
       </c>
       <c r="F32" s="28">
         <v>2</v>
       </c>
       <c r="G32" s="28">
-        <v>6</v>
+        <v>8.625</v>
       </c>
       <c r="H32" s="28">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I32" s="28">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="30">
         <v>43959</v>
       </c>
       <c r="C33" s="28">
-        <v>4</v>
-      </c>
-      <c r="D33" s="28">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="D33" s="31">
+        <v>10</v>
       </c>
       <c r="E33" s="28">
         <v>12</v>
       </c>
       <c r="F33" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" s="28">
         <v>6</v>
       </c>
       <c r="H33" s="28">
-        <v>7.75</v>
+        <v>8</v>
       </c>
       <c r="I33" s="28">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J33" s="22"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="27">
-        <v>43952</v>
+        <v>30</v>
+      </c>
+      <c r="B34" s="30">
+        <v>43959</v>
       </c>
       <c r="C34" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34" s="28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="28">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F34" s="28">
         <v>1</v>
       </c>
       <c r="G34" s="28">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H34" s="28">
-        <v>4.125</v>
+        <v>7.75</v>
       </c>
       <c r="I34" s="28">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" s="27">
         <v>43952</v>
       </c>
       <c r="C35" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35" s="28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E35" s="28">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F35" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35" s="28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="28">
-        <v>5.125</v>
+        <v>4.125</v>
       </c>
       <c r="I35" s="28">
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="J35" s="22"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B36" s="27">
         <v>43952</v>
       </c>
       <c r="C36" s="28">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="28">
-        <v>3.125</v>
+        <v>4</v>
       </c>
       <c r="E36" s="28">
         <v>12</v>
       </c>
-      <c r="F36" s="34" t="s">
-        <v>62</v>
+      <c r="F36" s="28">
+        <v>2</v>
       </c>
       <c r="G36" s="28">
         <v>6</v>
       </c>
-      <c r="H36" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="34" t="s">
-        <v>62</v>
+      <c r="H36" s="28">
+        <v>5.125</v>
+      </c>
+      <c r="I36" s="28">
+        <v>4.75</v>
       </c>
       <c r="J36" s="22"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B37" s="27">
         <v>43952</v>
       </c>
       <c r="C37" s="28">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D37" s="28">
-        <v>4</v>
+        <v>3.125</v>
       </c>
       <c r="E37" s="28">
         <v>12</v>
       </c>
-      <c r="F37" s="28">
-        <v>2</v>
+      <c r="F37" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="G37" s="28">
         <v>6</v>
       </c>
-      <c r="H37" s="28">
-        <v>7</v>
-      </c>
-      <c r="I37" s="28">
-        <v>7</v>
+      <c r="H37" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I37" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="J37" s="22"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B38" s="27">
-        <v>43958</v>
+        <v>43952</v>
       </c>
       <c r="C38" s="28">
         <v>4</v>
       </c>
       <c r="D38" s="28">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="E38" s="28">
         <v>12</v>
@@ -3368,185 +3374,215 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B39" s="27">
         <v>43958</v>
       </c>
       <c r="C39" s="28">
-        <v>5.75</v>
+        <v>4</v>
       </c>
       <c r="D39" s="28">
-        <v>5.75</v>
+        <v>4.25</v>
       </c>
       <c r="E39" s="28">
-        <v>10.75</v>
-      </c>
-      <c r="F39" s="29">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="F39" s="28">
+        <v>2</v>
       </c>
       <c r="G39" s="28">
-        <v>5.375</v>
+        <v>6</v>
       </c>
       <c r="H39" s="28">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="I39" s="28">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="J39" s="22"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B40" s="27">
         <v>43958</v>
       </c>
       <c r="C40" s="28">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="D40" s="28">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="E40" s="28">
-        <v>12</v>
-      </c>
-      <c r="F40" s="28">
-        <v>3.5</v>
+        <v>10.75</v>
+      </c>
+      <c r="F40" s="29">
+        <v>1</v>
       </c>
       <c r="G40" s="28">
-        <v>6</v>
+        <v>5.375</v>
       </c>
       <c r="H40" s="28">
-        <v>2.75</v>
+        <v>8.5</v>
       </c>
       <c r="I40" s="28">
-        <v>2.5</v>
+        <v>8.5</v>
       </c>
       <c r="J40" s="22"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" s="27">
         <v>43958</v>
       </c>
       <c r="C41" s="28">
-        <v>28</v>
+        <v>6.5</v>
       </c>
       <c r="D41" s="28">
-        <v>87</v>
+        <v>6.5</v>
       </c>
       <c r="E41" s="28">
-        <v>8</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>62</v>
+        <v>12</v>
+      </c>
+      <c r="F41" s="28">
+        <v>3.5</v>
       </c>
       <c r="G41" s="28">
-        <v>4</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="34" t="s">
-        <v>62</v>
+        <v>6</v>
+      </c>
+      <c r="H41" s="28">
+        <v>2.75</v>
+      </c>
+      <c r="I41" s="28">
+        <v>2.5</v>
       </c>
       <c r="J41" s="22"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="27">
         <v>43958</v>
       </c>
       <c r="C42" s="28">
-        <v>9.5</v>
+        <v>28</v>
       </c>
       <c r="D42" s="28">
-        <v>8.5</v>
+        <v>87</v>
       </c>
       <c r="E42" s="28">
         <v>8</v>
       </c>
-      <c r="F42" s="28">
-        <v>2</v>
+      <c r="F42" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="G42" s="28">
         <v>4</v>
       </c>
-      <c r="H42" s="28">
-        <v>8.5</v>
-      </c>
-      <c r="I42" s="28">
-        <v>9.25</v>
+      <c r="H42" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="J42" s="22"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="27">
         <v>43958</v>
       </c>
       <c r="C43" s="28">
-        <v>5.25</v>
+        <v>9.5</v>
       </c>
       <c r="D43" s="28">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="E43" s="28">
-        <v>14.5</v>
+        <v>8</v>
       </c>
       <c r="F43" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" s="28">
-        <v>7.25</v>
+        <v>4</v>
       </c>
       <c r="H43" s="28">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="I43" s="28">
-        <v>4.75</v>
+        <v>9.25</v>
       </c>
       <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="27">
         <v>43958</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="28">
+        <v>5.25</v>
+      </c>
+      <c r="D44" s="28">
+        <v>5</v>
+      </c>
+      <c r="E44" s="28">
+        <v>14.5</v>
+      </c>
+      <c r="F44" s="28">
+        <v>1</v>
+      </c>
+      <c r="G44" s="28">
+        <v>7.25</v>
+      </c>
+      <c r="H44" s="28">
+        <v>5</v>
+      </c>
+      <c r="I44" s="28">
+        <v>4.75</v>
+      </c>
+      <c r="J44" s="22"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="27">
+        <v>43958</v>
+      </c>
+      <c r="C45" s="24">
         <v>21.25</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D45" s="24">
         <v>20.75</v>
       </c>
-      <c r="E44" s="24">
+      <c r="E45" s="24">
         <v>11.5</v>
       </c>
-      <c r="F44" s="34" t="s">
+      <c r="F45" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G45" s="24">
         <v>5.75</v>
       </c>
-      <c r="H44" s="34" t="s">
+      <c r="H45" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I44" s="34" t="s">
+      <c r="I45" s="34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>